<commit_message>
averages bar chart added, demo made
</commit_message>
<xml_diff>
--- a/averages.xlsx
+++ b/averages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lover\Desktop\Josh\a. School\Year 3\C\DS 3010\Case Study 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56329DF7-D998-473D-BD76-02BD6AB3A0BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5608EE51-B8BA-4734-9C07-597EF030EA27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11808" yWindow="2409" windowWidth="13471" windowHeight="12999" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="14374" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Sanders</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Candidate</t>
   </si>
 </sst>
 </file>
@@ -79,7 +82,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,13 +121,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC611"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -150,12 +165,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFC611"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -432,73 +454,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.40100000000000002</v>
-      </c>
-      <c r="C2">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="C2" s="2">
         <v>0.42299999999999999</v>
       </c>
-      <c r="D2">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="D2" s="1">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="E2" s="1">
         <f>AVERAGE(B2:D2)</f>
-        <v>0.40433333333333338</v>
+        <v>0.48166666666666663</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="C3">
-        <v>0.42299999999999999</v>
-      </c>
-      <c r="D3">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="A3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="E3" s="2">
         <f>AVERAGE(B3:D3)</f>
-        <v>0.48166666666666663</v>
+        <v>0.4413333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>0.39700000000000002</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.41799999999999998</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.49099999999999999</v>
       </c>
       <c r="E4" s="3">
@@ -507,78 +533,81 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.372</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="E5" s="4">
+        <f>AVERAGE(B5:D5)</f>
+        <v>0.40733333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="E6" s="5">
+        <f>AVERAGE(B6:D6)</f>
+        <v>0.40433333333333338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E7" s="6">
+        <f>AVERAGE(B7:D7)</f>
+        <v>0.37166666666666665</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B8" s="7">
         <v>0.248</v>
       </c>
-      <c r="C5">
+      <c r="C8" s="7">
         <v>0.313</v>
       </c>
-      <c r="D5">
+      <c r="D8" s="7">
         <v>0.32800000000000001</v>
       </c>
-      <c r="E5" s="6">
-        <f>AVERAGE(B5:D5)</f>
+      <c r="E8" s="7">
+        <f>AVERAGE(B8:D8)</f>
         <v>0.29633333333333334</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>0.33100000000000002</v>
-      </c>
-      <c r="C6">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="D6">
-        <v>0.43099999999999999</v>
-      </c>
-      <c r="E6" s="7">
-        <f>AVERAGE(B6:D6)</f>
-        <v>0.37166666666666665</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0.41099999999999998</v>
-      </c>
-      <c r="C7">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="D7">
-        <v>0.50700000000000001</v>
-      </c>
-      <c r="E7" s="2">
-        <f>AVERAGE(B7:D7)</f>
-        <v>0.4413333333333333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>0.372</v>
-      </c>
-      <c r="C8">
-        <v>0.39300000000000002</v>
-      </c>
-      <c r="D8">
-        <v>0.45700000000000002</v>
-      </c>
-      <c r="E8" s="4">
-        <f>AVERAGE(B8:D8)</f>
-        <v>0.40733333333333333</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:E8">
+    <sortCondition descending="1" ref="E2:E8"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>